<commit_message>
update RDBES dota Model to v1.19.18
</commit_message>
<xml_diff>
--- a/data-raw/dataFormat/RDBES Data Model VD SL.xlsx
+++ b/data-raw/dataFormat/RDBES Data Model VD SL.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665FF0DF-D877-401F-A1C5-523736BCAF50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CC67E4-8630-4FF2-AE6C-A9F7310BD81C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="131">
   <si>
     <t>Hide</t>
   </si>
@@ -452,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,12 +468,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -540,9 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -840,7 +831,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -848,7 +839,7 @@
     <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.265625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="21.265625" style="18" customWidth="1"/>
     <col min="12" max="12" width="41.265625" customWidth="1"/>
     <col min="13" max="13" width="39.265625" customWidth="1"/>
   </cols>
@@ -1159,13 +1150,13 @@
       <c r="G9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="7" t="s">
         <v>128</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="7" t="s">
         <v>129</v>
       </c>
       <c r="K9" s="7"/>
@@ -1201,7 +1192,7 @@
       <c r="J10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="7" t="s">
         <v>123</v>
       </c>
       <c r="L10" s="7" t="s">
@@ -1331,7 +1322,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1341,9 +1332,10 @@
     <col min="6" max="6" width="17.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.1328125" style="2"/>
-    <col min="11" max="11" width="20.3984375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="20.3984375" style="18" customWidth="1"/>
     <col min="12" max="12" width="42.1328125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.1328125" style="2"/>
+    <col min="13" max="13" width="25.796875" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
@@ -1383,7 +1375,7 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1414,11 +1406,11 @@
         <v>15</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="20"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1449,7 +1441,7 @@
       <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1486,7 +1478,7 @@
       <c r="L4" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1521,7 +1513,7 @@
       <c r="L5" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1556,11 +1548,11 @@
       <c r="L6" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
@@ -1593,7 +1585,7 @@
       <c r="L7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1630,7 +1622,7 @@
       <c r="L8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="14" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1667,7 +1659,7 @@
       <c r="L9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1704,7 +1696,7 @@
       <c r="L10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1719,7 +1711,7 @@
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
     </row>
@@ -1734,7 +1726,7 @@
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
     </row>
@@ -1751,7 +1743,7 @@
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
-      <c r="K13" s="21"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
     </row>
@@ -1768,7 +1760,7 @@
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
-      <c r="K14" s="21"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
     </row>

</xml_diff>